<commit_message>
Cambio en query de version
</commit_message>
<xml_diff>
--- a/SimulacionMonteCarlo.xlsx
+++ b/SimulacionMonteCarlo.xlsx
@@ -460,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN11"/>
+  <dimension ref="A1:AI11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -582,40 +582,25 @@
         <v>27</v>
       </c>
       <c r="AC1" t="n" s="0">
-        <v>2032.0</v>
+        <v>2025.0</v>
       </c>
       <c r="AD1" t="n" s="0">
-        <v>2033.0</v>
+        <v>2026.0</v>
       </c>
       <c r="AE1" t="n" s="0">
-        <v>2025.0</v>
+        <v>2027.0</v>
       </c>
       <c r="AF1" t="n" s="0">
-        <v>2026.0</v>
+        <v>2028.0</v>
       </c>
       <c r="AG1" t="n" s="0">
-        <v>2027.0</v>
+        <v>2029.0</v>
       </c>
       <c r="AH1" t="n" s="0">
-        <v>2028.0</v>
+        <v>2030.0</v>
       </c>
       <c r="AI1" t="n" s="0">
-        <v>2029.0</v>
-      </c>
-      <c r="AJ1" t="n" s="0">
-        <v>2030.0</v>
-      </c>
-      <c r="AK1" t="n" s="0">
         <v>2031.0</v>
-      </c>
-      <c r="AL1" t="n" s="0">
-        <v>2034.0</v>
-      </c>
-      <c r="AM1" t="n" s="0">
-        <v>2035.0</v>
-      </c>
-      <c r="AN1" t="n" s="0">
-        <v>2036.0</v>
       </c>
     </row>
     <row r="2">
@@ -626,79 +611,70 @@
         <v>28</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>0.7427713798807951</v>
+        <v>0.3098472576134373</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>54.15129619940916</v>
+        <v>13.991309423144147</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.8355096696425163</v>
+        <v>0.44921425610235444</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>6.0965590014873685</v>
+        <v>4.533117506634735</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>0.7973744467189187</v>
+        <v>0.11203545540483906</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>11.437201750315191</v>
+        <v>19.053533985050784</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>0.5396237037402373</v>
+        <v>0.3236779242955993</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>5.071837809612097</v>
+        <v>4.187630361158099</v>
       </c>
       <c r="K2" t="n" s="0">
-        <v>1.2707182320441988</v>
+        <v>0.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>80.69178054664201</v>
+        <v>40.89660253322243</v>
       </c>
       <c r="M2" t="n" s="0">
-        <v>13.658860000000004</v>
+        <v>6.712729765247914</v>
       </c>
       <c r="N2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O2" t="n" s="0">
-        <v>36.140423747512244</v>
+        <v>24.64797916795166</v>
       </c>
       <c r="P2" t="n" s="0">
-        <v>7.589632848784616</v>
-      </c>
-      <c r="R2" t="n" s="0">
-        <v>40.33731318156061</v>
+        <v>4.760927013914146</v>
+      </c>
+      <c r="S2" t="n" s="0">
+        <v>0.12434000638417936</v>
       </c>
       <c r="U2" t="n" s="0">
-        <v>6.347542897639724</v>
+        <v>1.9135738597845742</v>
       </c>
       <c r="AC2" t="n" s="0">
-        <v>12.404167935500725</v>
+        <v>7.684685525355785</v>
       </c>
       <c r="AD2" t="n" s="0">
-        <v>4.5015865589422015</v>
+        <v>9.731867898577992</v>
       </c>
       <c r="AE2" t="n" s="0">
-        <v>14.574950786212012</v>
+        <v>7.877603141142188</v>
       </c>
       <c r="AF2" t="n" s="0">
-        <v>25.634011361996436</v>
+        <v>6.39552661826541</v>
       </c>
       <c r="AG2" t="n" s="0">
-        <v>22.702197765826156</v>
+        <v>5.161665822817412</v>
       </c>
       <c r="AH2" t="n" s="0">
-        <v>20.163332728169976</v>
-      </c>
-      <c r="AI2" t="n" s="0">
-        <v>17.806171949645</v>
-      </c>
-      <c r="AJ2" t="n" s="0">
-        <v>15.769644139756057</v>
-      </c>
-      <c r="AK2" t="n" s="0">
-        <v>13.96603812418541</v>
+        <v>1.1377540229870373</v>
       </c>
     </row>
     <row r="3">
@@ -706,85 +682,76 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>0.0</v>
+        <v>0.626905982688153</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>0.0</v>
+        <v>18.54833131530631</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>0.0</v>
+        <v>0.6141799310810776</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>0.0</v>
+        <v>4.879068365292783</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>0.0</v>
+        <v>0.2844052614570731</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>0.0</v>
+        <v>23.558597043302584</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>0.0</v>
+        <v>0.38840529491019377</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>0.0</v>
+        <v>4.37592255710402</v>
       </c>
       <c r="K3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>0.0</v>
+        <v>40.89660253322243</v>
       </c>
       <c r="M3" t="n" s="0">
-        <v>0.0</v>
+        <v>6.712729765247914</v>
       </c>
       <c r="N3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O3" t="n" s="0">
-        <v>0.0</v>
+        <v>20.908271362249845</v>
       </c>
       <c r="P3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Q3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R3" t="n" s="0">
-        <v>0.0</v>
+        <v>4.652707236873812</v>
       </c>
       <c r="S3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="T3" t="n" s="0">
-        <v>0.0</v>
+        <v>0.13856526013904508</v>
       </c>
       <c r="U3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="V3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="W3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="X3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Y3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Z3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="AA3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="AB3" t="n" s="0">
-        <v>0.0</v>
+        <v>2.0380884322468473</v>
+      </c>
+      <c r="AC3" t="n" s="0">
+        <v>9.58234354836637</v>
+      </c>
+      <c r="AD3" t="n" s="0">
+        <v>12.701576563571773</v>
+      </c>
+      <c r="AE3" t="n" s="0">
+        <v>9.709263322813344</v>
+      </c>
+      <c r="AF3" t="n" s="0">
+        <v>7.444332487296188</v>
+      </c>
+      <c r="AG3" t="n" s="0">
+        <v>5.673402269791736</v>
+      </c>
+      <c r="AH3" t="n" s="0">
+        <v>4.336828290405922</v>
+      </c>
+      <c r="AI3" t="n" s="0">
+        <v>1.1110842095523146</v>
       </c>
     </row>
     <row r="4">
@@ -792,76 +759,85 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>0.40874794656270363</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>26.898297529375817</v>
+        <v>0.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>0.24588701548592629</v>
+        <v>0.0</v>
       </c>
       <c r="F4" t="n" s="0">
-        <v>4.560339062188827</v>
+        <v>0.0</v>
       </c>
       <c r="G4" t="n" s="0">
-        <v>0.6194607807705028</v>
+        <v>0.0</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>10.673107075989712</v>
+        <v>0.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>0.6160833389337974</v>
+        <v>0.0</v>
       </c>
       <c r="J4" t="n" s="0">
-        <v>5.545864962259442</v>
+        <v>0.0</v>
       </c>
       <c r="K4" t="n" s="0">
-        <v>1.2707182320441988</v>
+        <v>0.0</v>
       </c>
       <c r="L4" t="n" s="0">
-        <v>80.69178054664201</v>
+        <v>0.0</v>
       </c>
       <c r="M4" t="n" s="0">
-        <v>13.658860000000004</v>
+        <v>0.0</v>
       </c>
       <c r="N4" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O4" t="n" s="0">
-        <v>38.74005645601165</v>
+        <v>0.0</v>
       </c>
       <c r="P4" t="n" s="0">
-        <v>9.391168036525901</v>
+        <v>0.0</v>
+      </c>
+      <c r="Q4" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="R4" t="n" s="0">
-        <v>39.196331034653234</v>
+        <v>0.0</v>
+      </c>
+      <c r="S4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T4" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="U4" t="n" s="0">
-        <v>6.875963677903694</v>
-      </c>
-      <c r="AE4" t="n" s="0">
-        <v>9.790144936978336</v>
-      </c>
-      <c r="AF4" t="n" s="0">
-        <v>14.944211188209245</v>
-      </c>
-      <c r="AG4" t="n" s="0">
-        <v>13.349199526429638</v>
-      </c>
-      <c r="AH4" t="n" s="0">
-        <v>11.958497683178237</v>
-      </c>
-      <c r="AI4" t="n" s="0">
-        <v>10.65171850089621</v>
-      </c>
-      <c r="AJ4" t="n" s="0">
-        <v>9.514849179862551</v>
-      </c>
-      <c r="AK4" t="n" s="0">
-        <v>2.792646346495258</v>
+        <v>0.0</v>
+      </c>
+      <c r="V4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA4" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB4" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -872,88 +848,70 @@
         <v>28</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.8922473347943757</v>
+        <v>0.4119562988806706</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>86.21429144895252</v>
+        <v>15.372378638261628</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.4142443120677163</v>
+        <v>0.1290372605914789</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>5.073748838629455</v>
+        <v>3.5848113578451217</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>0.8149488374652952</v>
+        <v>0.623676865310719</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>11.528687134615918</v>
+        <v>30.4652459094422</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>0.5173832626870674</v>
+        <v>0.1794821517741436</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>4.944051828250899</v>
+        <v>3.727949948656502</v>
       </c>
       <c r="K5" t="n" s="0">
-        <v>1.2707182320441988</v>
+        <v>0.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>80.69178054664201</v>
+        <v>40.89660253322243</v>
       </c>
       <c r="M5" t="n" s="0">
-        <v>13.658860000000004</v>
+        <v>6.712729765247914</v>
       </c>
       <c r="N5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O5" t="n" s="0">
-        <v>41.0929803350018</v>
+        <v>23.629399349728683</v>
       </c>
       <c r="P5" t="n" s="0">
-        <v>8.963783215388416</v>
-      </c>
-      <c r="R5" t="n" s="0">
-        <v>39.47692355901074</v>
+        <v>5.347910277410832</v>
+      </c>
+      <c r="S5" t="n" s="0">
+        <v>0.1379780605991107</v>
       </c>
       <c r="U5" t="n" s="0">
-        <v>6.028303839495143</v>
+        <v>2.0393696365289284</v>
       </c>
       <c r="AC5" t="n" s="0">
-        <v>17.8606574047285</v>
+        <v>8.232880552138775</v>
       </c>
       <c r="AD5" t="n" s="0">
-        <v>15.756376765653444</v>
+        <v>12.81476225915908</v>
       </c>
       <c r="AE5" t="n" s="0">
-        <v>13.196714380334335</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>36.21169980623586</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>32.858030244826054</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>29.15328861131619</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>25.718549374118865</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>22.753538281214983</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>20.130354040718643</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>13.939873384589944</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>7.6884623169098845</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.012846614627199165</v>
+        <v>8.910713424195865</v>
+      </c>
+      <c r="AF5" t="n" s="0">
+        <v>6.215405692272639</v>
+      </c>
+      <c r="AG5" t="n" s="0">
+        <v>4.308403032003664</v>
+      </c>
+      <c r="AH5" t="n" s="0">
+        <v>1.401373596615181</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Cambios de parametros de montecarlos
</commit_message>
<xml_diff>
--- a/SimulacionMonteCarlo.xlsx
+++ b/SimulacionMonteCarlo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="30">
   <si>
     <t>Iteración</t>
   </si>
@@ -98,10 +98,10 @@
     <t>buquetaQuerenta</t>
   </si>
   <si>
-    <t>Éxito</t>
+    <t>Fracaso</t>
   </si>
   <si>
-    <t>Fracaso</t>
+    <t>Éxito</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AI11"/>
+  <dimension ref="A1:AJ51"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -582,24 +582,27 @@
         <v>27</v>
       </c>
       <c r="AC1" t="n" s="0">
+        <v>2032.0</v>
+      </c>
+      <c r="AD1" t="n" s="0">
         <v>2025.0</v>
       </c>
-      <c r="AD1" t="n" s="0">
+      <c r="AE1" t="n" s="0">
         <v>2026.0</v>
       </c>
-      <c r="AE1" t="n" s="0">
+      <c r="AF1" t="n" s="0">
         <v>2027.0</v>
       </c>
-      <c r="AF1" t="n" s="0">
+      <c r="AG1" t="n" s="0">
         <v>2028.0</v>
       </c>
-      <c r="AG1" t="n" s="0">
+      <c r="AH1" t="n" s="0">
         <v>2029.0</v>
       </c>
-      <c r="AH1" t="n" s="0">
+      <c r="AI1" t="n" s="0">
         <v>2030.0</v>
       </c>
-      <c r="AI1" t="n" s="0">
+      <c r="AJ1" t="n" s="0">
         <v>2031.0</v>
       </c>
     </row>
@@ -611,70 +614,82 @@
         <v>28</v>
       </c>
       <c r="C2" t="n" s="0">
-        <v>0.3098472576134373</v>
+        <v>0.0</v>
       </c>
       <c r="D2" t="n" s="0">
-        <v>13.991309423144147</v>
+        <v>0.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.44921425610235444</v>
+        <v>0.0</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>4.533117506634735</v>
+        <v>0.0</v>
       </c>
       <c r="G2" t="n" s="0">
-        <v>0.11203545540483906</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>19.053533985050784</v>
+        <v>0.0</v>
       </c>
       <c r="I2" t="n" s="0">
-        <v>0.3236779242955993</v>
+        <v>0.0</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>4.187630361158099</v>
+        <v>0.0</v>
       </c>
       <c r="K2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>40.89660253322243</v>
+        <v>0.0</v>
       </c>
       <c r="M2" t="n" s="0">
-        <v>6.712729765247914</v>
+        <v>0.0</v>
       </c>
       <c r="N2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O2" t="n" s="0">
-        <v>24.64797916795166</v>
+        <v>0.0</v>
       </c>
       <c r="P2" t="n" s="0">
-        <v>4.760927013914146</v>
+        <v>0.0</v>
+      </c>
+      <c r="Q2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R2" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="S2" t="n" s="0">
-        <v>0.12434000638417936</v>
+        <v>0.0</v>
+      </c>
+      <c r="T2" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="U2" t="n" s="0">
-        <v>1.9135738597845742</v>
-      </c>
-      <c r="AC2" t="n" s="0">
-        <v>7.684685525355785</v>
-      </c>
-      <c r="AD2" t="n" s="0">
-        <v>9.731867898577992</v>
-      </c>
-      <c r="AE2" t="n" s="0">
-        <v>7.877603141142188</v>
-      </c>
-      <c r="AF2" t="n" s="0">
-        <v>6.39552661826541</v>
-      </c>
-      <c r="AG2" t="n" s="0">
-        <v>5.161665822817412</v>
-      </c>
-      <c r="AH2" t="n" s="0">
-        <v>1.1377540229870373</v>
+        <v>0.0</v>
+      </c>
+      <c r="V2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA2" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB2" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -685,73 +700,82 @@
         <v>28</v>
       </c>
       <c r="C3" t="n" s="0">
-        <v>0.626905982688153</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n" s="0">
-        <v>18.54833131530631</v>
+        <v>0.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>0.6141799310810776</v>
+        <v>0.0</v>
       </c>
       <c r="F3" t="n" s="0">
-        <v>4.879068365292783</v>
+        <v>0.0</v>
       </c>
       <c r="G3" t="n" s="0">
-        <v>0.2844052614570731</v>
+        <v>0.0</v>
       </c>
       <c r="H3" t="n" s="0">
-        <v>23.558597043302584</v>
+        <v>0.0</v>
       </c>
       <c r="I3" t="n" s="0">
-        <v>0.38840529491019377</v>
+        <v>0.0</v>
       </c>
       <c r="J3" t="n" s="0">
-        <v>4.37592255710402</v>
+        <v>0.0</v>
       </c>
       <c r="K3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="L3" t="n" s="0">
-        <v>40.89660253322243</v>
+        <v>0.0</v>
       </c>
       <c r="M3" t="n" s="0">
-        <v>6.712729765247914</v>
+        <v>0.0</v>
       </c>
       <c r="N3" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O3" t="n" s="0">
-        <v>20.908271362249845</v>
+        <v>0.0</v>
       </c>
       <c r="P3" t="n" s="0">
-        <v>4.652707236873812</v>
+        <v>0.0</v>
+      </c>
+      <c r="Q3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R3" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="S3" t="n" s="0">
-        <v>0.13856526013904508</v>
+        <v>0.0</v>
+      </c>
+      <c r="T3" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="U3" t="n" s="0">
-        <v>2.0380884322468473</v>
-      </c>
-      <c r="AC3" t="n" s="0">
-        <v>9.58234354836637</v>
-      </c>
-      <c r="AD3" t="n" s="0">
-        <v>12.701576563571773</v>
-      </c>
-      <c r="AE3" t="n" s="0">
-        <v>9.709263322813344</v>
-      </c>
-      <c r="AF3" t="n" s="0">
-        <v>7.444332487296188</v>
-      </c>
-      <c r="AG3" t="n" s="0">
-        <v>5.673402269791736</v>
-      </c>
-      <c r="AH3" t="n" s="0">
-        <v>4.336828290405922</v>
-      </c>
-      <c r="AI3" t="n" s="0">
-        <v>1.1110842095523146</v>
+        <v>0.0</v>
+      </c>
+      <c r="V3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA3" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB3" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -759,7 +783,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="n" s="0">
         <v>0.0</v>
@@ -848,70 +872,82 @@
         <v>28</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>0.4119562988806706</v>
+        <v>0.0</v>
       </c>
       <c r="D5" t="n" s="0">
-        <v>15.372378638261628</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>0.1290372605914789</v>
+        <v>0.0</v>
       </c>
       <c r="F5" t="n" s="0">
-        <v>3.5848113578451217</v>
+        <v>0.0</v>
       </c>
       <c r="G5" t="n" s="0">
-        <v>0.623676865310719</v>
+        <v>0.0</v>
       </c>
       <c r="H5" t="n" s="0">
-        <v>30.4652459094422</v>
+        <v>0.0</v>
       </c>
       <c r="I5" t="n" s="0">
-        <v>0.1794821517741436</v>
+        <v>0.0</v>
       </c>
       <c r="J5" t="n" s="0">
-        <v>3.727949948656502</v>
+        <v>0.0</v>
       </c>
       <c r="K5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="L5" t="n" s="0">
-        <v>40.89660253322243</v>
+        <v>0.0</v>
       </c>
       <c r="M5" t="n" s="0">
-        <v>6.712729765247914</v>
+        <v>0.0</v>
       </c>
       <c r="N5" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O5" t="n" s="0">
-        <v>23.629399349728683</v>
+        <v>0.0</v>
       </c>
       <c r="P5" t="n" s="0">
-        <v>5.347910277410832</v>
+        <v>0.0</v>
+      </c>
+      <c r="Q5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R5" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="S5" t="n" s="0">
-        <v>0.1379780605991107</v>
+        <v>0.0</v>
+      </c>
+      <c r="T5" t="n" s="0">
+        <v>0.0</v>
       </c>
       <c r="U5" t="n" s="0">
-        <v>2.0393696365289284</v>
-      </c>
-      <c r="AC5" t="n" s="0">
-        <v>8.232880552138775</v>
-      </c>
-      <c r="AD5" t="n" s="0">
-        <v>12.81476225915908</v>
-      </c>
-      <c r="AE5" t="n" s="0">
-        <v>8.910713424195865</v>
-      </c>
-      <c r="AF5" t="n" s="0">
-        <v>6.215405692272639</v>
-      </c>
-      <c r="AG5" t="n" s="0">
-        <v>4.308403032003664</v>
-      </c>
-      <c r="AH5" t="n" s="0">
-        <v>1.401373596615181</v>
+        <v>0.0</v>
+      </c>
+      <c r="V5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA5" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB5" t="n" s="0">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -919,7 +955,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="n" s="0">
         <v>0.0</v>
@@ -1005,7 +1041,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" t="n" s="0">
         <v>0.0</v>
@@ -1091,7 +1127,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="n" s="0">
         <v>0.0</v>
@@ -1177,7 +1213,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="n" s="0">
         <v>0.0</v>
@@ -1263,7 +1299,7 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="n" s="0">
         <v>0.0</v>
@@ -1349,84 +1385,3500 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB11" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB12" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="D11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="E11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="F11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="H11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="I11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="J11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="K11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="L11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="M11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="N11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="O11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="P11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Q11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="R11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="S11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="T11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="U11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="V11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="W11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="X11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Y11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="Z11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="AA11" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="AB11" t="n" s="0">
+      <c r="C14" t="n" s="0">
+        <v>0.5604229014532316</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>43.1861611234936</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>0.06029927161272297</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>0.07699059888235116</v>
+      </c>
+      <c r="H14" t="n" s="0">
+        <v>13.760755583092488</v>
+      </c>
+      <c r="I14" t="n" s="0">
+        <v>0.6925906691726565</v>
+      </c>
+      <c r="J14" t="n" s="0">
+        <v>6.440673014103648</v>
+      </c>
+      <c r="K14" t="n" s="0">
+        <v>1.578089026611146</v>
+      </c>
+      <c r="L14" t="n" s="0">
+        <v>46.12954363586871</v>
+      </c>
+      <c r="M14" t="n" s="0">
+        <v>6.1403357201652</v>
+      </c>
+      <c r="N14" t="n" s="0">
+        <v>1.18971136701173</v>
+      </c>
+      <c r="O14" t="n" s="0">
+        <v>23.661022380864203</v>
+      </c>
+      <c r="P14" t="n" s="0">
+        <v>4.034077910551162</v>
+      </c>
+      <c r="S14" t="n" s="0">
+        <v>0.21922432411328427</v>
+      </c>
+      <c r="U14" t="n" s="0">
+        <v>3.9944628064777414</v>
+      </c>
+      <c r="AC14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AD14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AE14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AF14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AG14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AI14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AJ14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n" s="0">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>0.2203049378963977</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>17.646383241762813</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>0.684347095153962</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="0">
+        <v>0.7148297300430564</v>
+      </c>
+      <c r="H15" t="n" s="0">
+        <v>35.82096476061769</v>
+      </c>
+      <c r="I15" t="n" s="0">
+        <v>0.6117526896646449</v>
+      </c>
+      <c r="J15" t="n" s="0">
+        <v>5.61206199678156</v>
+      </c>
+      <c r="K15" t="n" s="0">
+        <v>1.578089026611146</v>
+      </c>
+      <c r="L15" t="n" s="0">
+        <v>46.12954363586871</v>
+      </c>
+      <c r="M15" t="n" s="0">
+        <v>6.1403357201652</v>
+      </c>
+      <c r="N15" t="n" s="0">
+        <v>1.25881095098099</v>
+      </c>
+      <c r="O15" t="n" s="0">
+        <v>21.77637225145294</v>
+      </c>
+      <c r="P15" t="n" s="0">
+        <v>4.317882096595318</v>
+      </c>
+      <c r="S15" t="n" s="0">
+        <v>0.23771629768266542</v>
+      </c>
+      <c r="U15" t="n" s="0">
+        <v>3.396213678405216</v>
+      </c>
+      <c r="AD15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AE15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AF15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AG15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AI15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AJ15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n" s="0">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n" s="0">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB17" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n" s="0">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB18" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n" s="0">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB19" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n" s="0">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB20" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n" s="0">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB21" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB22" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n" s="0">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB23" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n" s="0">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB24" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n" s="0">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C25" t="n" s="0">
+        <v>0.255599626137631</v>
+      </c>
+      <c r="D25" t="n" s="0">
+        <v>19.71210762222595</v>
+      </c>
+      <c r="E25" t="n" s="0">
+        <v>0.2458023114708866</v>
+      </c>
+      <c r="F25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G25" t="n" s="0">
+        <v>0.5996087230043737</v>
+      </c>
+      <c r="H25" t="n" s="0">
+        <v>33.03017681264261</v>
+      </c>
+      <c r="I25" t="n" s="0">
+        <v>0.04747144686920649</v>
+      </c>
+      <c r="J25" t="n" s="0">
+        <v>1.6455832171905758</v>
+      </c>
+      <c r="K25" t="n" s="0">
+        <v>1.578089026611146</v>
+      </c>
+      <c r="L25" t="n" s="0">
+        <v>46.12954363586871</v>
+      </c>
+      <c r="M25" t="n" s="0">
+        <v>6.1403357201652</v>
+      </c>
+      <c r="N25" t="n" s="0">
+        <v>1.1441489691688744</v>
+      </c>
+      <c r="O25" t="n" s="0">
+        <v>22.23045964783659</v>
+      </c>
+      <c r="P25" t="n" s="0">
+        <v>4.123480398311534</v>
+      </c>
+      <c r="S25" t="n" s="0">
+        <v>0.21567929403288877</v>
+      </c>
+      <c r="U25" t="n" s="0">
+        <v>3.461026531726772</v>
+      </c>
+      <c r="AD25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AE25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AF25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AG25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AH25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AI25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AJ25" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n" s="0">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB26" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n" s="0">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB27" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n" s="0">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB28" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n" s="0">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB29" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n" s="0">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB30" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB31" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n" s="0">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB32" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n" s="0">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n" s="0">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n" s="0">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n" s="0">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n" s="0">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n" s="0">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n" s="0">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n" s="0">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n" s="0">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n" s="0">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB42" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n" s="0">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB43" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n" s="0">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB44" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n" s="0">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB45" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n" s="0">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB46" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n" s="0">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB47" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n" s="0">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB48" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n" s="0">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB49" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n" s="0">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB50" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n" s="0">
+        <v>50.0</v>
+      </c>
+      <c r="B51" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="F51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="R51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="S51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="T51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="U51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="V51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="W51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="X51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Y51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Z51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AA51" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="AB51" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>